<commit_message>
Added EXO to draft_list and line_distributions
</commit_message>
<xml_diff>
--- a/app/assets/spreadsheets/Idol-Draft-Test-Server-Ranks.xlsx
+++ b/app/assets/spreadsheets/Idol-Draft-Test-Server-Ranks.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adhityavadivel/IdolDraft/app/assets/spreadsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c3d7be37c56f4b2c/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12ED2727-9747-5745-BCF8-437AC9ED32BA}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="239" documentId="11_35C13A2D796FF2CD3640ACB35C8EA54943F2538E" xr6:coauthVersionLast="33" xr6:coauthVersionMax="34" xr10:uidLastSave="{B0D4F8BA-DC51-DF4C-A87F-AFED6462BBFC}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="22680" windowHeight="15480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="318">
   <si>
     <t>                     Test Server Ranks</t>
   </si>
@@ -947,6 +947,42 @@
   </si>
   <si>
     <t>Gorilla</t>
+  </si>
+  <si>
+    <t>Chen</t>
+  </si>
+  <si>
+    <t>D.O</t>
+  </si>
+  <si>
+    <t>Baekhyun</t>
+  </si>
+  <si>
+    <t>Suho</t>
+  </si>
+  <si>
+    <t>Xiumin</t>
+  </si>
+  <si>
+    <t>Chanyeol</t>
+  </si>
+  <si>
+    <t>Kai</t>
+  </si>
+  <si>
+    <t>Sehun</t>
+  </si>
+  <si>
+    <t>Lay</t>
+  </si>
+  <si>
+    <t>Kris</t>
+  </si>
+  <si>
+    <t>Tao</t>
+  </si>
+  <si>
+    <t>Luhan</t>
   </si>
 </sst>
 </file>
@@ -1021,7 +1057,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="72">
+  <fills count="73">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1446,6 +1482,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFE958F1"/>
         <bgColor rgb="FFC2A6E0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor rgb="FFA8D08D"/>
       </patternFill>
     </fill>
   </fills>
@@ -1519,7 +1561,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1713,17 +1755,30 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="72" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="66" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2081,8 +2136,8 @@
   </sheetPr>
   <dimension ref="A1:Z103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="141" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G92" sqref="G92"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="141" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2303,7 +2358,7 @@
     </row>
     <row r="7" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>25</v>
@@ -2351,7 +2406,7 @@
     </row>
     <row r="8" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>22</v>
@@ -2497,7 +2552,7 @@
     </row>
     <row r="11" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="B11" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>37</v>
@@ -2545,7 +2600,7 @@
     </row>
     <row r="12" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>34</v>
@@ -2593,7 +2648,7 @@
     </row>
     <row r="13" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>36</v>
@@ -2985,7 +3040,7 @@
     </row>
     <row r="21" spans="2:26" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="2">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>54</v>
@@ -3035,7 +3090,7 @@
     </row>
     <row r="22" spans="2:26" ht="16" x14ac:dyDescent="0.2">
       <c r="B22" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>53</v>
@@ -3469,31 +3524,31 @@
         <v>27</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D31" s="85" t="s">
-        <v>42</v>
+        <v>306</v>
+      </c>
+      <c r="D31" s="105" t="s">
+        <v>177</v>
       </c>
       <c r="E31" s="40" t="s">
         <v>20</v>
       </c>
       <c r="F31" s="44"/>
       <c r="G31" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H31" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I31" s="44">
         <v>17</v>
       </c>
-      <c r="I31" s="73">
-        <v>25</v>
-      </c>
-      <c r="J31" s="48">
-        <v>20</v>
-      </c>
-      <c r="K31" s="48">
+      <c r="J31" s="44">
         <v>18</v>
       </c>
-      <c r="L31" s="80">
+      <c r="K31" s="44">
+        <v>28</v>
+      </c>
+      <c r="L31" s="98">
         <f>AVERAGE(I31:K31)</f>
         <v>21</v>
       </c>
@@ -3502,104 +3557,102 @@
       <c r="B32" s="2">
         <v>28</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D32" s="102" t="s">
-        <v>38</v>
-      </c>
-      <c r="E32" s="95" t="s">
-        <v>14</v>
-      </c>
-      <c r="F32" s="45" t="s">
-        <v>15</v>
-      </c>
+      <c r="C32" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="85" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" s="44"/>
       <c r="G32" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I32" s="44">
-        <v>15</v>
-      </c>
-      <c r="J32" s="44">
-        <v>19</v>
-      </c>
-      <c r="K32" s="44">
-        <v>28</v>
+        <v>16</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I32" s="73">
+        <v>25</v>
+      </c>
+      <c r="J32" s="48">
+        <v>20</v>
+      </c>
+      <c r="K32" s="48">
+        <v>18</v>
       </c>
       <c r="L32" s="80">
         <f>AVERAGE(I32:K32)</f>
-        <v>20.666666666666668</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="2:12" ht="16" x14ac:dyDescent="0.2">
       <c r="B33" s="2">
-        <v>30</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D33" s="90" t="s">
-        <v>63</v>
-      </c>
-      <c r="E33" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" s="102" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33" s="95" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="42" t="s">
+      <c r="F33" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="G33" s="2" t="s">
-        <v>64</v>
+      <c r="G33" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="I33" s="44">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J33" s="44">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="K33" s="44">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L33" s="80">
         <f>AVERAGE(I33:K33)</f>
-        <v>20.333333333333332</v>
+        <v>20.666666666666668</v>
       </c>
     </row>
     <row r="34" spans="2:12" ht="16" x14ac:dyDescent="0.2">
       <c r="B34" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D34" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="E34" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="90" t="s">
+        <v>63</v>
+      </c>
+      <c r="E34" s="71" t="s">
         <v>14</v>
       </c>
       <c r="F34" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G34" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="H34" s="7" t="s">
-        <v>21</v>
+      <c r="G34" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="I34" s="44">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="J34" s="44">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K34" s="44">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="L34" s="80">
         <f>AVERAGE(I34:K34)</f>
@@ -3611,29 +3664,31 @@
         <v>31</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D35" s="91" t="s">
-        <v>72</v>
-      </c>
-      <c r="E35" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="F35" s="44"/>
-      <c r="G35" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="H35" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="E35" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H35" s="7" t="s">
         <v>21</v>
       </c>
       <c r="I35" s="44">
+        <v>11</v>
+      </c>
+      <c r="J35" s="44">
         <v>16</v>
       </c>
-      <c r="J35" s="44">
-        <v>19</v>
-      </c>
       <c r="K35" s="44">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="L35" s="80">
         <f>AVERAGE(I35:K35)</f>
@@ -3642,66 +3697,66 @@
     </row>
     <row r="36" spans="2:12" ht="16" x14ac:dyDescent="0.2">
       <c r="B36" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D36" s="90" t="s">
-        <v>63</v>
-      </c>
-      <c r="E36" s="71" t="s">
-        <v>14</v>
+        <v>71</v>
+      </c>
+      <c r="D36" s="91" t="s">
+        <v>72</v>
+      </c>
+      <c r="E36" s="40" t="s">
+        <v>20</v>
       </c>
       <c r="F36" s="44"/>
       <c r="G36" s="2" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I36" s="44">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J36" s="44">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K36" s="44">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L36" s="80">
         <f>AVERAGE(I36:K36)</f>
-        <v>20</v>
+        <v>20.333333333333332</v>
       </c>
     </row>
     <row r="37" spans="2:12" ht="16" x14ac:dyDescent="0.2">
       <c r="B37" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D37" s="84" t="s">
-        <v>35</v>
-      </c>
-      <c r="E37" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" s="90" t="s">
+        <v>63</v>
+      </c>
+      <c r="E37" s="71" t="s">
         <v>14</v>
       </c>
       <c r="F37" s="44"/>
-      <c r="G37" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H37" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I37" s="105">
+      <c r="G37" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I37" s="2">
+        <v>13</v>
+      </c>
+      <c r="J37" s="2">
         <v>22</v>
       </c>
-      <c r="J37" s="108">
-        <v>19</v>
-      </c>
-      <c r="K37" s="108">
-        <v>19</v>
+      <c r="K37" s="2">
+        <v>25</v>
       </c>
       <c r="L37" s="80">
         <f>AVERAGE(I37:K37)</f>
@@ -3710,68 +3765,66 @@
     </row>
     <row r="38" spans="2:12" ht="16" x14ac:dyDescent="0.2">
       <c r="B38" s="2">
+        <v>34</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D38" s="84" t="s">
         <v>35</v>
       </c>
-      <c r="C38" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D38" s="101" t="s">
-        <v>45</v>
-      </c>
-      <c r="E38" s="41" t="s">
-        <v>20</v>
+      <c r="E38" s="38" t="s">
+        <v>14</v>
       </c>
       <c r="F38" s="44"/>
-      <c r="G38" s="2" t="s">
+      <c r="G38" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H38" s="2" t="s">
+      <c r="H38" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I38" s="44">
-        <v>14</v>
-      </c>
-      <c r="J38" s="44">
-        <v>13</v>
-      </c>
-      <c r="K38" s="44">
-        <v>33</v>
-      </c>
-      <c r="L38" s="98">
+      <c r="I38" s="73">
+        <v>22</v>
+      </c>
+      <c r="J38" s="48">
+        <v>19</v>
+      </c>
+      <c r="K38" s="48">
+        <v>19</v>
+      </c>
+      <c r="L38" s="80">
         <f>AVERAGE(I38:K38)</f>
         <v>20</v>
       </c>
     </row>
     <row r="39" spans="2:12" ht="16" x14ac:dyDescent="0.2">
       <c r="B39" s="2">
-        <v>34</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D39" s="99" t="s">
-        <v>26</v>
-      </c>
-      <c r="E39" s="93" t="s">
-        <v>20</v>
-      </c>
-      <c r="F39" s="45" t="s">
-        <v>15</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D39" s="101" t="s">
+        <v>45</v>
+      </c>
+      <c r="E39" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="F39" s="44"/>
       <c r="G39" s="2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I39" s="107">
-        <v>23</v>
-      </c>
-      <c r="J39" s="107">
-        <v>17</v>
-      </c>
-      <c r="K39" s="107">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="I39" s="2">
+        <v>14</v>
+      </c>
+      <c r="J39" s="2">
+        <v>13</v>
+      </c>
+      <c r="K39" s="2">
+        <v>33</v>
       </c>
       <c r="L39" s="98">
         <f>AVERAGE(I39:K39)</f>
@@ -3780,68 +3833,68 @@
     </row>
     <row r="40" spans="2:12" ht="16" x14ac:dyDescent="0.2">
       <c r="B40" s="2">
-        <v>37</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D40" s="101" t="s">
-        <v>45</v>
-      </c>
-      <c r="E40" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="F40" s="44"/>
+        <v>36</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D40" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="E40" s="93" t="s">
+        <v>20</v>
+      </c>
+      <c r="F40" s="45" t="s">
+        <v>15</v>
+      </c>
       <c r="G40" s="2" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I40" s="44">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J40" s="44">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K40" s="44">
-        <v>13</v>
-      </c>
-      <c r="L40" s="80">
+        <v>20</v>
+      </c>
+      <c r="L40" s="98">
         <f>AVERAGE(I40:K40)</f>
-        <v>19.666666666666668</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="2:12" ht="16" x14ac:dyDescent="0.2">
       <c r="B41" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D41" s="91" t="s">
-        <v>72</v>
-      </c>
-      <c r="E41" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="F41" s="42" t="s">
-        <v>15</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="D41" s="101" t="s">
+        <v>45</v>
+      </c>
+      <c r="E41" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="F41" s="44"/>
       <c r="G41" s="2" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>21</v>
       </c>
       <c r="I41" s="44">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="J41" s="44">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K41" s="44">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L41" s="80">
         <f>AVERAGE(I41:K41)</f>
@@ -3853,15 +3906,17 @@
         <v>38</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D42" s="91" t="s">
         <v>72</v>
       </c>
-      <c r="E42" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="F42" s="44"/>
+      <c r="E42" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="F42" s="42" t="s">
+        <v>15</v>
+      </c>
       <c r="G42" s="2" t="s">
         <v>73</v>
       </c>
@@ -3869,17 +3924,17 @@
         <v>21</v>
       </c>
       <c r="I42" s="44">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J42" s="44">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="K42" s="44">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="L42" s="80">
         <f>AVERAGE(I42:K42)</f>
-        <v>19.333333333333332</v>
+        <v>19.666666666666668</v>
       </c>
     </row>
     <row r="43" spans="2:12" ht="16" x14ac:dyDescent="0.2">
@@ -3887,33 +3942,31 @@
         <v>39</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D43" s="100" t="s">
-        <v>82</v>
-      </c>
-      <c r="E43" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="F43" s="42" t="s">
-        <v>15</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="D43" s="91" t="s">
+        <v>72</v>
+      </c>
+      <c r="E43" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="F43" s="44"/>
       <c r="G43" s="2" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>21</v>
       </c>
       <c r="I43" s="44">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="J43" s="44">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="K43" s="44">
-        <v>16</v>
-      </c>
-      <c r="L43" s="98">
+        <v>20</v>
+      </c>
+      <c r="L43" s="80">
         <f>AVERAGE(I43:K43)</f>
         <v>19.333333333333332</v>
       </c>
@@ -3923,7 +3976,7 @@
         <v>40</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D44" s="100" t="s">
         <v>82</v>
@@ -3931,7 +3984,9 @@
       <c r="E44" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="F44" s="44"/>
+      <c r="F44" s="42" t="s">
+        <v>15</v>
+      </c>
       <c r="G44" s="2" t="s">
         <v>56</v>
       </c>
@@ -3939,51 +3994,51 @@
         <v>21</v>
       </c>
       <c r="I44" s="44">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J44" s="44">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K44" s="44">
         <v>16</v>
       </c>
-      <c r="L44" s="80">
+      <c r="L44" s="98">
         <f>AVERAGE(I44:K44)</f>
-        <v>19</v>
+        <v>19.333333333333332</v>
       </c>
     </row>
     <row r="45" spans="2:12" ht="16" x14ac:dyDescent="0.2">
       <c r="B45" s="2">
         <v>41</v>
       </c>
-      <c r="C45" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D45" s="99" t="s">
-        <v>26</v>
-      </c>
-      <c r="E45" s="93" t="s">
+      <c r="C45" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D45" s="100" t="s">
+        <v>82</v>
+      </c>
+      <c r="E45" s="40" t="s">
         <v>20</v>
       </c>
       <c r="F45" s="44"/>
       <c r="G45" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I45" s="44">
+        <v>14</v>
+      </c>
+      <c r="J45" s="44">
         <v>27</v>
       </c>
-      <c r="H45" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I45" s="44">
-        <v>21</v>
-      </c>
-      <c r="J45" s="44">
-        <v>15</v>
-      </c>
       <c r="K45" s="44">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L45" s="80">
         <f>AVERAGE(I45:K45)</f>
-        <v>18.666666666666668</v>
+        <v>19</v>
       </c>
     </row>
     <row r="46" spans="2:12" ht="16" x14ac:dyDescent="0.2">
@@ -3991,67 +4046,67 @@
         <v>42</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D46" s="100" t="s">
-        <v>82</v>
+        <v>308</v>
+      </c>
+      <c r="D46" s="105" t="s">
+        <v>177</v>
       </c>
       <c r="E46" s="40" t="s">
         <v>20</v>
       </c>
       <c r="F46" s="44"/>
-      <c r="G46" s="2" t="s">
-        <v>56</v>
+      <c r="G46" s="7" t="s">
+        <v>64</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>21</v>
       </c>
       <c r="I46" s="44">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J46" s="44">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K46" s="44">
-        <v>18</v>
-      </c>
-      <c r="L46" s="80">
+        <v>21</v>
+      </c>
+      <c r="L46" s="98">
         <f>AVERAGE(I46:K46)</f>
-        <v>18.333333333333332</v>
+        <v>18.666666666666668</v>
       </c>
     </row>
     <row r="47" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="2">
         <v>43</v>
       </c>
-      <c r="C47" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D47" s="91" t="s">
-        <v>72</v>
-      </c>
-      <c r="E47" s="40" t="s">
+      <c r="C47" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D47" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="E47" s="93" t="s">
         <v>20</v>
       </c>
       <c r="F47" s="44"/>
       <c r="G47" s="2" t="s">
-        <v>73</v>
+        <v>27</v>
       </c>
       <c r="H47" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I47" s="44">
         <v>21</v>
       </c>
-      <c r="I47" s="44">
-        <v>10</v>
-      </c>
       <c r="J47" s="44">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="K47" s="44">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="L47" s="80">
         <f>AVERAGE(I47:K47)</f>
-        <v>17.666666666666668</v>
+        <v>18.666666666666668</v>
       </c>
     </row>
     <row r="48" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4059,33 +4114,33 @@
         <v>44</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D48" s="92" t="s">
-        <v>19</v>
-      </c>
-      <c r="E48" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="D48" s="100" t="s">
+        <v>82</v>
+      </c>
+      <c r="E48" s="40" t="s">
         <v>20</v>
       </c>
       <c r="F48" s="44"/>
       <c r="G48" s="2" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="H48" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I48" s="2">
-        <v>17</v>
-      </c>
-      <c r="J48" s="2">
+      <c r="I48" s="107">
         <v>22</v>
       </c>
-      <c r="K48" s="2">
-        <v>12</v>
+      <c r="J48" s="107">
+        <v>15</v>
+      </c>
+      <c r="K48" s="107">
+        <v>18</v>
       </c>
       <c r="L48" s="80">
         <f>AVERAGE(I48:K48)</f>
-        <v>17</v>
+        <v>18.333333333333332</v>
       </c>
     </row>
     <row r="49" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4093,171 +4148,171 @@
         <v>45</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D49" s="92" t="s">
-        <v>19</v>
-      </c>
-      <c r="E49" s="71" t="s">
-        <v>14</v>
+        <v>86</v>
+      </c>
+      <c r="D49" s="91" t="s">
+        <v>72</v>
+      </c>
+      <c r="E49" s="40" t="s">
+        <v>20</v>
       </c>
       <c r="F49" s="44"/>
       <c r="G49" s="2" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="H49" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I49" s="2">
-        <v>15</v>
-      </c>
-      <c r="J49" s="2">
-        <v>13</v>
-      </c>
-      <c r="K49" s="2">
-        <v>22</v>
+      <c r="I49" s="107">
+        <v>10</v>
+      </c>
+      <c r="J49" s="107">
+        <v>26</v>
+      </c>
+      <c r="K49" s="107">
+        <v>17</v>
       </c>
       <c r="L49" s="80">
         <f>AVERAGE(I49:K49)</f>
-        <v>16.666666666666668</v>
+        <v>17.666666666666668</v>
       </c>
     </row>
     <row r="50" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="2">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D50" s="89" t="s">
-        <v>32</v>
-      </c>
-      <c r="E50" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="F50" s="46" t="s">
-        <v>47</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="D50" s="92" t="s">
+        <v>19</v>
+      </c>
+      <c r="E50" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="F50" s="44"/>
       <c r="G50" s="2" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="H50" s="2" t="s">
         <v>21</v>
       </c>
       <c r="I50" s="44">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="J50" s="44">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="K50" s="44">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L50" s="80">
         <f>AVERAGE(I50:K50)</f>
-        <v>16.333333333333332</v>
+        <v>17</v>
       </c>
     </row>
     <row r="51" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D51" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="E51" s="40" t="s">
-        <v>20</v>
+        <v>88</v>
+      </c>
+      <c r="D51" s="92" t="s">
+        <v>19</v>
+      </c>
+      <c r="E51" s="71" t="s">
+        <v>14</v>
       </c>
       <c r="F51" s="44"/>
-      <c r="G51" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="H51" s="7" t="s">
+      <c r="G51" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H51" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I51" s="106">
+      <c r="I51" s="2">
+        <v>15</v>
+      </c>
+      <c r="J51" s="2">
+        <v>13</v>
+      </c>
+      <c r="K51" s="2">
         <v>22</v>
-      </c>
-      <c r="J51" s="106">
-        <v>18</v>
-      </c>
-      <c r="K51" s="106">
-        <v>9</v>
       </c>
       <c r="L51" s="80">
         <f>AVERAGE(I51:K51)</f>
-        <v>16.333333333333332</v>
+        <v>16.666666666666668</v>
       </c>
     </row>
     <row r="52" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="2">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D52" s="101" t="s">
-        <v>45</v>
-      </c>
-      <c r="E52" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="F52" s="44"/>
+        <v>90</v>
+      </c>
+      <c r="D52" s="89" t="s">
+        <v>32</v>
+      </c>
+      <c r="E52" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="F52" s="46" t="s">
+        <v>47</v>
+      </c>
       <c r="G52" s="2" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="H52" s="2" t="s">
         <v>21</v>
       </c>
       <c r="I52" s="44">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="J52" s="44">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K52" s="44">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="L52" s="80">
         <f>AVERAGE(I52:K52)</f>
-        <v>16</v>
+        <v>16.333333333333332</v>
       </c>
     </row>
     <row r="53" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B53" s="2">
-        <v>48</v>
-      </c>
-      <c r="C53" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="D53" s="87" t="s">
-        <v>23</v>
+        <v>49</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D53" s="86" t="s">
+        <v>49</v>
       </c>
       <c r="E53" s="40" t="s">
         <v>20</v>
       </c>
       <c r="F53" s="44"/>
       <c r="G53" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I53" s="44">
-        <v>15</v>
-      </c>
-      <c r="J53" s="44">
-        <v>16</v>
-      </c>
-      <c r="K53" s="44">
-        <v>17</v>
+        <v>50</v>
+      </c>
+      <c r="H53" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I53" s="36">
+        <v>22</v>
+      </c>
+      <c r="J53" s="36">
+        <v>18</v>
+      </c>
+      <c r="K53" s="36">
+        <v>9</v>
       </c>
       <c r="L53" s="80">
         <f>AVERAGE(I53:K53)</f>
-        <v>16</v>
+        <v>16.333333333333332</v>
       </c>
     </row>
     <row r="54" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4265,103 +4320,101 @@
         <v>50</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D54" s="89" t="s">
-        <v>32</v>
-      </c>
-      <c r="E54" s="38" t="s">
-        <v>14</v>
+        <v>92</v>
+      </c>
+      <c r="D54" s="101" t="s">
+        <v>45</v>
+      </c>
+      <c r="E54" s="41" t="s">
+        <v>20</v>
       </c>
       <c r="F54" s="44"/>
       <c r="G54" s="2" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="H54" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I54" s="2">
-        <v>11</v>
-      </c>
-      <c r="J54" s="2">
-        <v>16</v>
-      </c>
-      <c r="K54" s="2">
-        <v>19</v>
+      <c r="I54" s="107">
+        <v>15</v>
+      </c>
+      <c r="J54" s="107">
+        <v>13</v>
+      </c>
+      <c r="K54" s="107">
+        <v>20</v>
       </c>
       <c r="L54" s="80">
         <f>AVERAGE(I54:K54)</f>
-        <v>15.333333333333334</v>
+        <v>16</v>
       </c>
     </row>
     <row r="55" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="2">
-        <v>52</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D55" s="99" t="s">
-        <v>26</v>
-      </c>
-      <c r="E55" s="93" t="s">
+        <v>51</v>
+      </c>
+      <c r="C55" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D55" s="87" t="s">
+        <v>23</v>
+      </c>
+      <c r="E55" s="40" t="s">
         <v>20</v>
       </c>
       <c r="F55" s="44"/>
-      <c r="G55" s="2" t="s">
-        <v>27</v>
+      <c r="G55" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>17</v>
       </c>
       <c r="I55" s="107">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J55" s="107">
         <v>16</v>
       </c>
       <c r="K55" s="107">
-        <v>13</v>
-      </c>
-      <c r="L55" s="98">
+        <v>17</v>
+      </c>
+      <c r="L55" s="80">
         <f>AVERAGE(I55:K55)</f>
-        <v>15.333333333333334</v>
+        <v>16</v>
       </c>
     </row>
     <row r="56" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B56" s="2">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D56" s="90" t="s">
-        <v>63</v>
+        <v>307</v>
+      </c>
+      <c r="D56" s="105" t="s">
+        <v>177</v>
       </c>
       <c r="E56" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="F56" s="46" t="s">
-        <v>47</v>
-      </c>
-      <c r="G56" s="2" t="s">
+      <c r="F56" s="44"/>
+      <c r="G56" s="7" t="s">
         <v>64</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I56" s="44">
+        <v>15</v>
+      </c>
+      <c r="J56" s="44">
         <v>14</v>
       </c>
-      <c r="J56" s="44">
-        <v>19</v>
-      </c>
       <c r="K56" s="44">
-        <v>13</v>
-      </c>
-      <c r="L56" s="80">
+        <v>18</v>
+      </c>
+      <c r="L56" s="98">
         <f>AVERAGE(I56:K56)</f>
-        <v>15.333333333333334</v>
+        <v>15.666666666666666</v>
       </c>
     </row>
     <row r="57" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4369,33 +4422,33 @@
         <v>53</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D57" s="84" t="s">
-        <v>35</v>
-      </c>
-      <c r="E57" s="40" t="s">
-        <v>20</v>
+        <v>93</v>
+      </c>
+      <c r="D57" s="89" t="s">
+        <v>32</v>
+      </c>
+      <c r="E57" s="38" t="s">
+        <v>14</v>
       </c>
       <c r="F57" s="44"/>
-      <c r="G57" s="7" t="s">
+      <c r="G57" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I57" s="44">
+        <v>11</v>
+      </c>
+      <c r="J57" s="44">
         <v>16</v>
       </c>
-      <c r="H57" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I57" s="72">
-        <v>8</v>
-      </c>
-      <c r="J57" s="48">
+      <c r="K57" s="44">
         <v>19</v>
-      </c>
-      <c r="K57" s="48">
-        <v>16</v>
       </c>
       <c r="L57" s="80">
         <f>AVERAGE(I57:K57)</f>
-        <v>14.333333333333334</v>
+        <v>15.333333333333334</v>
       </c>
     </row>
     <row r="58" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4403,103 +4456,103 @@
         <v>54</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D58" s="88" t="s">
-        <v>29</v>
-      </c>
-      <c r="E58" s="70" t="s">
-        <v>14</v>
+        <v>95</v>
+      </c>
+      <c r="D58" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="E58" s="93" t="s">
+        <v>20</v>
       </c>
       <c r="F58" s="44"/>
       <c r="G58" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>17</v>
       </c>
       <c r="I58" s="44">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="J58" s="44">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="K58" s="44">
-        <v>22</v>
-      </c>
-      <c r="L58" s="80">
+        <v>13</v>
+      </c>
+      <c r="L58" s="98">
         <f>AVERAGE(I58:K58)</f>
-        <v>13.666666666666666</v>
+        <v>15.333333333333334</v>
       </c>
     </row>
     <row r="59" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="2">
-        <v>56</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D59" s="99" t="s">
-        <v>26</v>
-      </c>
-      <c r="E59" s="95" t="s">
-        <v>14</v>
-      </c>
-      <c r="F59" s="96" t="s">
+        <v>55</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D59" s="90" t="s">
+        <v>63</v>
+      </c>
+      <c r="E59" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="F59" s="46" t="s">
         <v>47</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>17</v>
       </c>
       <c r="I59" s="44">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="J59" s="44">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="K59" s="44">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="L59" s="80">
         <f>AVERAGE(I59:K59)</f>
-        <v>12.666666666666666</v>
+        <v>15.333333333333334</v>
       </c>
     </row>
     <row r="60" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B60" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D60" s="83" t="s">
+        <v>311</v>
+      </c>
+      <c r="D60" s="105" t="s">
+        <v>177</v>
+      </c>
+      <c r="E60" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="F60" s="44"/>
+      <c r="G60" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I60" s="44">
+        <v>11</v>
+      </c>
+      <c r="J60" s="44">
         <v>13</v>
       </c>
-      <c r="E60" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="F60" s="44"/>
-      <c r="G60" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H60" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I60" s="73">
-        <v>12</v>
-      </c>
-      <c r="J60" s="48">
-        <v>11</v>
-      </c>
-      <c r="K60" s="48">
+      <c r="K60" s="44">
+        <v>21</v>
+      </c>
+      <c r="L60" s="98">
+        <f>AVERAGE(I60:K60)</f>
         <v>15</v>
-      </c>
-      <c r="L60" s="80">
-        <f>AVERAGE(I60:K60)</f>
-        <v>12.666666666666666</v>
       </c>
     </row>
     <row r="61" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4507,243 +4560,241 @@
         <v>57</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D61" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="E61" s="71" t="s">
-        <v>14</v>
+        <v>96</v>
+      </c>
+      <c r="D61" s="84" t="s">
+        <v>35</v>
+      </c>
+      <c r="E61" s="40" t="s">
+        <v>20</v>
       </c>
       <c r="F61" s="44"/>
       <c r="G61" s="7" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="H61" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I61" s="7">
-        <v>9</v>
-      </c>
-      <c r="J61" s="7">
-        <v>13</v>
-      </c>
-      <c r="K61" s="7">
-        <v>14</v>
+      <c r="I61" s="108">
+        <v>8</v>
+      </c>
+      <c r="J61" s="111">
+        <v>19</v>
+      </c>
+      <c r="K61" s="111">
+        <v>16</v>
       </c>
       <c r="L61" s="80">
         <f>AVERAGE(I61:K61)</f>
-        <v>12</v>
+        <v>14.333333333333334</v>
       </c>
     </row>
     <row r="62" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="2">
-        <v>62</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D62" s="100" t="s">
-        <v>82</v>
-      </c>
-      <c r="E62" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D62" s="88" t="s">
+        <v>29</v>
+      </c>
+      <c r="E62" s="70" t="s">
         <v>14</v>
       </c>
       <c r="F62" s="44"/>
       <c r="G62" s="2" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I62" s="107">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J62" s="107">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K62" s="107">
-        <v>13</v>
-      </c>
-      <c r="L62" s="98">
+        <v>22</v>
+      </c>
+      <c r="L62" s="80">
         <f>AVERAGE(I62:K62)</f>
-        <v>11.666666666666666</v>
+        <v>13.666666666666666</v>
       </c>
     </row>
     <row r="63" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B63" s="2">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D63" s="91" t="s">
-        <v>72</v>
-      </c>
-      <c r="E63" s="40" t="s">
-        <v>20</v>
+        <v>312</v>
+      </c>
+      <c r="D63" s="105" t="s">
+        <v>177</v>
+      </c>
+      <c r="E63" s="71" t="s">
+        <v>14</v>
       </c>
       <c r="F63" s="44"/>
-      <c r="G63" s="2" t="s">
-        <v>73</v>
+      <c r="G63" s="7" t="s">
+        <v>64</v>
       </c>
       <c r="H63" s="2" t="s">
         <v>21</v>
       </c>
       <c r="I63" s="2">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="J63" s="2">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="K63" s="2">
-        <v>13</v>
-      </c>
-      <c r="L63" s="80">
+        <v>21</v>
+      </c>
+      <c r="L63" s="98">
         <f>AVERAGE(I63:K63)</f>
-        <v>11.666666666666666</v>
+        <v>13.333333333333334</v>
       </c>
     </row>
     <row r="64" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B64" s="2">
-        <v>59</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D64" s="91" t="s">
-        <v>72</v>
-      </c>
-      <c r="E64" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="F64" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D64" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="E64" s="95" t="s">
+        <v>14</v>
+      </c>
+      <c r="F64" s="96" t="s">
         <v>47</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>73</v>
+        <v>27</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I64" s="2">
-        <v>15</v>
-      </c>
-      <c r="J64" s="2">
-        <v>9</v>
-      </c>
-      <c r="K64" s="2">
-        <v>11</v>
+        <v>17</v>
+      </c>
+      <c r="I64" s="107">
+        <v>20</v>
+      </c>
+      <c r="J64" s="107">
+        <v>8</v>
+      </c>
+      <c r="K64" s="107">
+        <v>10</v>
       </c>
       <c r="L64" s="80">
         <f>AVERAGE(I64:K64)</f>
-        <v>11.666666666666666</v>
+        <v>12.666666666666666</v>
       </c>
     </row>
     <row r="65" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B65" s="2">
-        <v>63</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D65" s="103" t="s">
-        <v>55</v>
+        <v>61</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D65" s="83" t="s">
+        <v>13</v>
       </c>
       <c r="E65" s="40" t="s">
         <v>20</v>
       </c>
       <c r="F65" s="44"/>
-      <c r="G65" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="H65" s="2" t="s">
+      <c r="G65" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H65" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I65" s="44">
+      <c r="I65" s="73">
+        <v>12</v>
+      </c>
+      <c r="J65" s="48">
         <v>11</v>
       </c>
-      <c r="J65" s="44">
-        <v>13</v>
-      </c>
-      <c r="K65" s="44">
-        <v>11</v>
+      <c r="K65" s="48">
+        <v>15</v>
       </c>
       <c r="L65" s="80">
         <f>AVERAGE(I65:K65)</f>
-        <v>11.666666666666666</v>
+        <v>12.666666666666666</v>
       </c>
     </row>
     <row r="66" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B66" s="2">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D66" s="89" t="s">
-        <v>32</v>
-      </c>
-      <c r="E66" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="F66" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H66" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D66" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="E66" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="F66" s="44"/>
+      <c r="G66" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H66" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I66" s="44">
+      <c r="I66" s="36">
+        <v>9</v>
+      </c>
+      <c r="J66" s="36">
         <v>13</v>
       </c>
-      <c r="J66" s="44">
-        <v>13</v>
-      </c>
-      <c r="K66" s="44">
-        <v>9</v>
+      <c r="K66" s="36">
+        <v>14</v>
       </c>
       <c r="L66" s="80">
         <f>AVERAGE(I66:K66)</f>
-        <v>11.666666666666666</v>
+        <v>12</v>
       </c>
     </row>
     <row r="67" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B67" s="2">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D67" s="100" t="s">
-        <v>82</v>
+        <v>309</v>
+      </c>
+      <c r="D67" s="105" t="s">
+        <v>177</v>
       </c>
       <c r="E67" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="F67" s="46" t="s">
-        <v>47</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>56</v>
+      <c r="F67" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="G67" s="7" t="s">
+        <v>64</v>
       </c>
       <c r="H67" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I67" s="107">
-        <v>11</v>
-      </c>
-      <c r="J67" s="107">
+      <c r="I67" s="2">
+        <v>9</v>
+      </c>
+      <c r="J67" s="2">
+        <v>15</v>
+      </c>
+      <c r="K67" s="2">
         <v>12</v>
       </c>
-      <c r="K67" s="107">
+      <c r="L67" s="98">
+        <f>AVERAGE(I67:K67)</f>
         <v>12</v>
-      </c>
-      <c r="L67" s="80">
-        <f>AVERAGE(I67:K67)</f>
-        <v>11.666666666666666</v>
       </c>
     </row>
     <row r="68" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4751,12 +4802,12 @@
         <v>64</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D68" s="100" t="s">
         <v>82</v>
       </c>
-      <c r="E68" s="38" t="s">
+      <c r="E68" s="71" t="s">
         <v>14</v>
       </c>
       <c r="F68" s="44"/>
@@ -4767,17 +4818,17 @@
         <v>21</v>
       </c>
       <c r="I68" s="44">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J68" s="44">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K68" s="44">
-        <v>12</v>
-      </c>
-      <c r="L68" s="80">
+        <v>13</v>
+      </c>
+      <c r="L68" s="98">
         <f>AVERAGE(I68:K68)</f>
-        <v>11.333333333333334</v>
+        <v>11.666666666666666</v>
       </c>
     </row>
     <row r="69" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4785,33 +4836,33 @@
         <v>65</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D69" s="103" t="s">
-        <v>55</v>
+        <v>103</v>
+      </c>
+      <c r="D69" s="91" t="s">
+        <v>72</v>
       </c>
       <c r="E69" s="40" t="s">
         <v>20</v>
       </c>
       <c r="F69" s="44"/>
-      <c r="G69" s="7" t="s">
-        <v>56</v>
+      <c r="G69" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I69" s="2">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="J69" s="2">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="K69" s="2">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="L69" s="80">
         <f>AVERAGE(I69:K69)</f>
-        <v>10.333333333333334</v>
+        <v>11.666666666666666</v>
       </c>
     </row>
     <row r="70" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4819,53 +4870,53 @@
         <v>66</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="D70" s="89" t="s">
-        <v>32</v>
+        <v>102</v>
+      </c>
+      <c r="D70" s="91" t="s">
+        <v>72</v>
       </c>
       <c r="E70" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="F70" s="44"/>
+      <c r="F70" s="46" t="s">
+        <v>47</v>
+      </c>
       <c r="G70" s="2" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="H70" s="2" t="s">
         <v>21</v>
       </c>
       <c r="I70" s="2">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="J70" s="2">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="K70" s="2">
         <v>11</v>
       </c>
       <c r="L70" s="80">
         <f>AVERAGE(I70:K70)</f>
-        <v>10</v>
+        <v>11.666666666666666</v>
       </c>
     </row>
     <row r="71" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B71" s="2">
         <v>67</v>
       </c>
-      <c r="C71" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="D71" s="87" t="s">
-        <v>23</v>
-      </c>
-      <c r="E71" s="71" t="s">
-        <v>14</v>
-      </c>
-      <c r="F71" s="46" t="s">
-        <v>47</v>
-      </c>
+      <c r="C71" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D71" s="103" t="s">
+        <v>55</v>
+      </c>
+      <c r="E71" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="F71" s="44"/>
       <c r="G71" s="7" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="H71" s="2" t="s">
         <v>17</v>
@@ -4874,64 +4925,68 @@
         <v>11</v>
       </c>
       <c r="J71" s="44">
+        <v>13</v>
+      </c>
+      <c r="K71" s="44">
         <v>11</v>
-      </c>
-      <c r="K71" s="44">
-        <v>7</v>
       </c>
       <c r="L71" s="80">
         <f>AVERAGE(I71:K71)</f>
-        <v>9.6666666666666661</v>
+        <v>11.666666666666666</v>
       </c>
     </row>
     <row r="72" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B72" s="2">
         <v>68</v>
       </c>
-      <c r="C72" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="D72" s="87" t="s">
-        <v>23</v>
+      <c r="C72" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D72" s="89" t="s">
+        <v>32</v>
       </c>
       <c r="E72" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="F72" s="44"/>
-      <c r="G72" s="7" t="s">
-        <v>24</v>
+      <c r="F72" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I72" s="2">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J72" s="2">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="K72" s="2">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="L72" s="80">
         <f>AVERAGE(I72:K72)</f>
-        <v>9.3333333333333339</v>
+        <v>11.666666666666666</v>
       </c>
     </row>
     <row r="73" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B73" s="2">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="D73" s="100" t="s">
         <v>82</v>
       </c>
-      <c r="E73" s="71" t="s">
-        <v>14</v>
-      </c>
-      <c r="F73" s="44"/>
+      <c r="E73" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="F73" s="46" t="s">
+        <v>47</v>
+      </c>
       <c r="G73" s="2" t="s">
         <v>56</v>
       </c>
@@ -4939,17 +4994,17 @@
         <v>21</v>
       </c>
       <c r="I73" s="44">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="J73" s="44">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="K73" s="44">
         <v>12</v>
       </c>
       <c r="L73" s="80">
         <f>AVERAGE(I73:K73)</f>
-        <v>9</v>
+        <v>11.666666666666666</v>
       </c>
     </row>
     <row r="74" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4957,33 +5012,33 @@
         <v>70</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D74" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="E74" s="71" t="s">
+        <v>107</v>
+      </c>
+      <c r="D74" s="100" t="s">
+        <v>82</v>
+      </c>
+      <c r="E74" s="38" t="s">
         <v>14</v>
       </c>
       <c r="F74" s="44"/>
-      <c r="G74" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="H74" s="7" t="s">
+      <c r="G74" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H74" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I74" s="106">
-        <v>9</v>
-      </c>
-      <c r="J74" s="106">
+      <c r="I74" s="107">
+        <v>14</v>
+      </c>
+      <c r="J74" s="107">
         <v>8</v>
       </c>
-      <c r="K74" s="106">
-        <v>10</v>
+      <c r="K74" s="107">
+        <v>12</v>
       </c>
       <c r="L74" s="80">
         <f>AVERAGE(I74:K74)</f>
-        <v>9</v>
+        <v>11.333333333333334</v>
       </c>
     </row>
     <row r="75" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4991,139 +5046,137 @@
         <v>71</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="D75" s="89" t="s">
-        <v>32</v>
+        <v>108</v>
+      </c>
+      <c r="D75" s="103" t="s">
+        <v>55</v>
       </c>
       <c r="E75" s="40" t="s">
         <v>20</v>
       </c>
       <c r="F75" s="44"/>
-      <c r="G75" s="2" t="s">
-        <v>33</v>
+      <c r="G75" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I75" s="44">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J75" s="44">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="K75" s="44">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="L75" s="80">
         <f>AVERAGE(I75:K75)</f>
-        <v>9</v>
+        <v>10.333333333333334</v>
       </c>
     </row>
     <row r="76" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B76" s="2">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="D76" s="86" t="s">
-        <v>49</v>
+        <v>109</v>
+      </c>
+      <c r="D76" s="89" t="s">
+        <v>32</v>
       </c>
       <c r="E76" s="40" t="s">
         <v>20</v>
       </c>
       <c r="F76" s="44"/>
-      <c r="G76" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="H76" s="7" t="s">
+      <c r="G76" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H76" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I76" s="36">
+      <c r="I76" s="44">
+        <v>6</v>
+      </c>
+      <c r="J76" s="44">
         <v>13</v>
       </c>
-      <c r="J76" s="36">
+      <c r="K76" s="44">
         <v>11</v>
-      </c>
-      <c r="K76" s="36">
-        <v>3</v>
       </c>
       <c r="L76" s="80">
         <f>AVERAGE(I76:K76)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="77" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B77" s="2">
         <v>73</v>
       </c>
-      <c r="C77" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D77" s="84" t="s">
-        <v>35</v>
-      </c>
-      <c r="E77" s="40" t="s">
-        <v>20</v>
+      <c r="C77" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="D77" s="87" t="s">
+        <v>23</v>
+      </c>
+      <c r="E77" s="71" t="s">
+        <v>14</v>
       </c>
       <c r="F77" s="46" t="s">
         <v>47</v>
       </c>
       <c r="G77" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H77" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I77" s="73">
-        <v>8</v>
-      </c>
-      <c r="J77" s="48">
-        <v>0</v>
-      </c>
-      <c r="K77" s="48">
+        <v>24</v>
+      </c>
+      <c r="H77" s="2" t="s">
         <v>17</v>
+      </c>
+      <c r="I77" s="44">
+        <v>11</v>
+      </c>
+      <c r="J77" s="44">
+        <v>11</v>
+      </c>
+      <c r="K77" s="44">
+        <v>7</v>
       </c>
       <c r="L77" s="80">
         <f>AVERAGE(I77:K77)</f>
-        <v>8.3333333333333339</v>
+        <v>9.6666666666666661</v>
       </c>
     </row>
     <row r="78" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B78" s="2">
         <v>74</v>
       </c>
-      <c r="C78" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="D78" s="92" t="s">
-        <v>19</v>
+      <c r="C78" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="D78" s="87" t="s">
+        <v>23</v>
       </c>
       <c r="E78" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="F78" s="46" t="s">
-        <v>47</v>
-      </c>
-      <c r="G78" s="2" t="s">
-        <v>16</v>
+      <c r="F78" s="44"/>
+      <c r="G78" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I78" s="44">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="J78" s="44">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K78" s="44">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="L78" s="80">
         <f>AVERAGE(I78:K78)</f>
-        <v>8</v>
+        <v>9.3333333333333339</v>
       </c>
     </row>
     <row r="79" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5131,33 +5184,33 @@
         <v>75</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="D79" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="E79" s="40" t="s">
-        <v>20</v>
+        <v>115</v>
+      </c>
+      <c r="D79" s="100" t="s">
+        <v>82</v>
+      </c>
+      <c r="E79" s="71" t="s">
+        <v>14</v>
       </c>
       <c r="F79" s="44"/>
-      <c r="G79" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="H79" s="7" t="s">
+      <c r="G79" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H79" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I79" s="36">
-        <v>13</v>
-      </c>
-      <c r="J79" s="36">
-        <v>6</v>
-      </c>
-      <c r="K79" s="36">
-        <v>3</v>
+      <c r="I79" s="44">
+        <v>7</v>
+      </c>
+      <c r="J79" s="44">
+        <v>8</v>
+      </c>
+      <c r="K79" s="44">
+        <v>12</v>
       </c>
       <c r="L79" s="80">
         <f>AVERAGE(I79:K79)</f>
-        <v>7.333333333333333</v>
+        <v>9</v>
       </c>
     </row>
     <row r="80" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5165,103 +5218,101 @@
         <v>76</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D80" s="103" t="s">
-        <v>55</v>
-      </c>
-      <c r="E80" s="40" t="s">
-        <v>20</v>
+        <v>113</v>
+      </c>
+      <c r="D80" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="E80" s="71" t="s">
+        <v>14</v>
       </c>
       <c r="F80" s="44"/>
       <c r="G80" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="H80" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I80" s="44">
-        <v>7</v>
-      </c>
-      <c r="J80" s="44">
-        <v>7</v>
-      </c>
-      <c r="K80" s="44">
-        <v>7</v>
-      </c>
-      <c r="L80" s="98">
+        <v>50</v>
+      </c>
+      <c r="H80" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I80" s="36">
+        <v>9</v>
+      </c>
+      <c r="J80" s="36">
+        <v>8</v>
+      </c>
+      <c r="K80" s="36">
+        <v>10</v>
+      </c>
+      <c r="L80" s="80">
         <f>AVERAGE(I80:K80)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="81" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B81" s="2">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D81" s="103" t="s">
-        <v>55</v>
-      </c>
-      <c r="E81" s="71" t="s">
-        <v>14</v>
+        <v>114</v>
+      </c>
+      <c r="D81" s="89" t="s">
+        <v>32</v>
+      </c>
+      <c r="E81" s="40" t="s">
+        <v>20</v>
       </c>
       <c r="F81" s="44"/>
-      <c r="G81" s="7" t="s">
-        <v>56</v>
+      <c r="G81" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I81" s="44">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J81" s="44">
+        <v>7</v>
+      </c>
+      <c r="K81" s="44">
+        <v>13</v>
+      </c>
+      <c r="L81" s="80">
+        <f>AVERAGE(I81:K81)</f>
         <v>9</v>
-      </c>
-      <c r="K81" s="44">
-        <v>6</v>
-      </c>
-      <c r="L81" s="98">
-        <f>AVERAGE(I81:K81)</f>
-        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="82" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B82" s="2">
-        <v>77</v>
-      </c>
-      <c r="C82" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="D82" s="87" t="s">
-        <v>23</v>
-      </c>
-      <c r="E82" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="F82" s="42" t="s">
-        <v>15</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D82" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="E82" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="F82" s="44"/>
       <c r="G82" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H82" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I82" s="44">
-        <v>8</v>
-      </c>
-      <c r="J82" s="44">
-        <v>4</v>
-      </c>
-      <c r="K82" s="44">
-        <v>8</v>
+        <v>50</v>
+      </c>
+      <c r="H82" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I82" s="36">
+        <v>13</v>
+      </c>
+      <c r="J82" s="36">
+        <v>11</v>
+      </c>
+      <c r="K82" s="36">
+        <v>3</v>
       </c>
       <c r="L82" s="80">
         <f>AVERAGE(I82:K82)</f>
-        <v>6.666666666666667</v>
+        <v>9</v>
       </c>
     </row>
     <row r="83" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5269,137 +5320,139 @@
         <v>79</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D83" s="101" t="s">
-        <v>45</v>
-      </c>
-      <c r="E83" s="41" t="s">
+        <v>310</v>
+      </c>
+      <c r="D83" s="105" t="s">
+        <v>177</v>
+      </c>
+      <c r="E83" s="40" t="s">
         <v>20</v>
       </c>
       <c r="F83" s="44"/>
-      <c r="G83" s="2" t="s">
-        <v>16</v>
+      <c r="G83" s="7" t="s">
+        <v>64</v>
       </c>
       <c r="H83" s="2" t="s">
         <v>21</v>
       </c>
       <c r="I83" s="44">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J83" s="44">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="K83" s="44">
+        <v>7</v>
+      </c>
+      <c r="L83" s="98">
+        <f>AVERAGE(I83:K83)</f>
         <v>9</v>
-      </c>
-      <c r="L83" s="80">
-        <f>AVERAGE(I83:K83)</f>
-        <v>6.333333333333333</v>
       </c>
     </row>
     <row r="84" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B84" s="2">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D84" s="103" t="s">
-        <v>55</v>
-      </c>
-      <c r="E84" s="71" t="s">
-        <v>14</v>
-      </c>
-      <c r="F84" s="44"/>
+        <v>116</v>
+      </c>
+      <c r="D84" s="84" t="s">
+        <v>35</v>
+      </c>
+      <c r="E84" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="F84" s="46" t="s">
+        <v>47</v>
+      </c>
       <c r="G84" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="H84" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H84" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I84" s="109">
+        <v>8</v>
+      </c>
+      <c r="J84" s="111">
+        <v>0</v>
+      </c>
+      <c r="K84" s="111">
         <v>17</v>
-      </c>
-      <c r="I84" s="2">
-        <v>3</v>
-      </c>
-      <c r="J84" s="2">
-        <v>9</v>
-      </c>
-      <c r="K84" s="2">
-        <v>6</v>
       </c>
       <c r="L84" s="80">
         <f>AVERAGE(I84:K84)</f>
-        <v>6</v>
+        <v>8.3333333333333339</v>
       </c>
     </row>
     <row r="85" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B85" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="D85" s="89" t="s">
-        <v>32</v>
+        <v>117</v>
+      </c>
+      <c r="D85" s="92" t="s">
+        <v>19</v>
       </c>
       <c r="E85" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="F85" s="44"/>
+      <c r="F85" s="46" t="s">
+        <v>47</v>
+      </c>
       <c r="G85" s="2" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="H85" s="2" t="s">
         <v>21</v>
       </c>
       <c r="I85" s="44">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="J85" s="44">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K85" s="44">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="L85" s="80">
         <f>AVERAGE(I85:K85)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="86" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B86" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D86" s="103" t="s">
-        <v>55</v>
+        <v>118</v>
+      </c>
+      <c r="D86" s="86" t="s">
+        <v>49</v>
       </c>
       <c r="E86" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="F86" s="46" t="s">
-        <v>47</v>
-      </c>
+      <c r="F86" s="44"/>
       <c r="G86" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="H86" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I86" s="107">
+        <v>50</v>
+      </c>
+      <c r="H86" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I86" s="110">
+        <v>13</v>
+      </c>
+      <c r="J86" s="110">
         <v>6</v>
       </c>
-      <c r="J86" s="107">
-        <v>5</v>
-      </c>
-      <c r="K86" s="107">
-        <v>7</v>
+      <c r="K86" s="110">
+        <v>3</v>
       </c>
       <c r="L86" s="80">
         <f>AVERAGE(I86:K86)</f>
-        <v>6</v>
+        <v>7.333333333333333</v>
       </c>
     </row>
     <row r="87" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5407,152 +5460,530 @@
         <v>83</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="D87" s="101" t="s">
-        <v>45</v>
-      </c>
-      <c r="E87" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="D87" s="103" t="s">
+        <v>55</v>
+      </c>
+      <c r="E87" s="40" t="s">
         <v>20</v>
       </c>
       <c r="F87" s="44"/>
-      <c r="G87" s="2" t="s">
-        <v>16</v>
+      <c r="G87" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I87" s="2">
-        <v>6</v>
-      </c>
-      <c r="J87" s="2">
-        <v>4</v>
-      </c>
-      <c r="K87" s="2">
-        <v>6</v>
+        <v>17</v>
+      </c>
+      <c r="I87" s="107">
+        <v>7</v>
+      </c>
+      <c r="J87" s="107">
+        <v>7</v>
+      </c>
+      <c r="K87" s="107">
+        <v>7</v>
       </c>
       <c r="L87" s="98">
         <f>AVERAGE(I87:K87)</f>
-        <v>5.333333333333333</v>
+        <v>7</v>
       </c>
     </row>
     <row r="88" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B88" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D88" s="103" t="s">
-        <v>55</v>
+        <v>315</v>
+      </c>
+      <c r="D88" s="105" t="s">
+        <v>177</v>
       </c>
       <c r="E88" s="71" t="s">
         <v>14</v>
       </c>
       <c r="F88" s="44"/>
       <c r="G88" s="7" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I88" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J88" s="2">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K88" s="2">
-        <v>6</v>
-      </c>
-      <c r="L88" s="80">
+        <v>20</v>
+      </c>
+      <c r="L88" s="98">
         <f>AVERAGE(I88:K88)</f>
-        <v>5</v>
+        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="89" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B89" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C89" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D89" s="103" t="s">
+        <v>55</v>
+      </c>
+      <c r="E89" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="F89" s="44"/>
+      <c r="G89" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H89" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I89" s="107">
+        <v>5</v>
+      </c>
+      <c r="J89" s="107">
+        <v>9</v>
+      </c>
+      <c r="K89" s="107">
+        <v>6</v>
+      </c>
+      <c r="L89" s="98">
+        <f>AVERAGE(I89:K89)</f>
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="90" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B90" s="2">
+        <v>86</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="D90" s="105" t="s">
+        <v>177</v>
+      </c>
+      <c r="E90" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="F90" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="G90" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H90" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I90" s="2">
+        <v>8</v>
+      </c>
+      <c r="J90" s="2">
+        <v>6</v>
+      </c>
+      <c r="K90" s="2">
+        <v>6</v>
+      </c>
+      <c r="L90" s="47">
+        <f>AVERAGE(I90:K90)</f>
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="91" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B91" s="2">
+        <v>87</v>
+      </c>
+      <c r="C91" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D91" s="87" t="s">
+        <v>23</v>
+      </c>
+      <c r="E91" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="F91" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="G91" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H91" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I91" s="107">
+        <v>8</v>
+      </c>
+      <c r="J91" s="107">
+        <v>4</v>
+      </c>
+      <c r="K91" s="107">
+        <v>8</v>
+      </c>
+      <c r="L91" s="112">
+        <f>AVERAGE(I91:K91)</f>
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="92" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B92" s="2">
+        <v>88</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="D92" s="105" t="s">
+        <v>177</v>
+      </c>
+      <c r="E92" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="F92" s="44"/>
+      <c r="G92" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H92" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I92" s="2">
+        <v>0</v>
+      </c>
+      <c r="J92" s="2">
+        <v>0</v>
+      </c>
+      <c r="K92" s="2">
+        <v>19</v>
+      </c>
+      <c r="L92" s="47">
+        <f>AVERAGE(I92:K92)</f>
+        <v>6.333333333333333</v>
+      </c>
+    </row>
+    <row r="93" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B93" s="2">
+        <v>89</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D93" s="101" t="s">
+        <v>45</v>
+      </c>
+      <c r="E93" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="F93" s="44"/>
+      <c r="G93" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H93" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I93" s="107">
+        <v>6</v>
+      </c>
+      <c r="J93" s="107">
+        <v>4</v>
+      </c>
+      <c r="K93" s="107">
+        <v>9</v>
+      </c>
+      <c r="L93" s="112">
+        <f>AVERAGE(I93:K93)</f>
+        <v>6.333333333333333</v>
+      </c>
+    </row>
+    <row r="94" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B94" s="2">
+        <v>90</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D94" s="103" t="s">
+        <v>55</v>
+      </c>
+      <c r="E94" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="F94" s="44"/>
+      <c r="G94" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H94" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I94" s="2">
+        <v>3</v>
+      </c>
+      <c r="J94" s="2">
+        <v>9</v>
+      </c>
+      <c r="K94" s="2">
+        <v>6</v>
+      </c>
+      <c r="L94" s="112">
+        <f>AVERAGE(I94:K94)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B95" s="2">
+        <v>91</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D95" s="89" t="s">
+        <v>32</v>
+      </c>
+      <c r="E95" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="F95" s="44"/>
+      <c r="G95" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H95" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I95" s="2">
+        <v>5</v>
+      </c>
+      <c r="J95" s="2">
+        <v>4</v>
+      </c>
+      <c r="K95" s="2">
+        <v>9</v>
+      </c>
+      <c r="L95" s="112">
+        <f>AVERAGE(I95:K95)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B96" s="2">
+        <v>92</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D96" s="103" t="s">
+        <v>55</v>
+      </c>
+      <c r="E96" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="F96" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="G96" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H96" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I96" s="107">
+        <v>6</v>
+      </c>
+      <c r="J96" s="107">
+        <v>5</v>
+      </c>
+      <c r="K96" s="107">
+        <v>7</v>
+      </c>
+      <c r="L96" s="112">
+        <f>AVERAGE(I96:K96)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B97" s="2">
+        <v>93</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="D97" s="105" t="s">
+        <v>177</v>
+      </c>
+      <c r="E97" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="F97" s="44"/>
+      <c r="G97" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H97" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I97" s="2">
+        <v>0</v>
+      </c>
+      <c r="J97" s="2">
+        <v>0</v>
+      </c>
+      <c r="K97" s="2">
+        <v>17</v>
+      </c>
+      <c r="L97" s="47">
+        <f>AVERAGE(I97:K97)</f>
+        <v>5.666666666666667</v>
+      </c>
+    </row>
+    <row r="98" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B98" s="2">
+        <v>94</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D98" s="101" t="s">
+        <v>45</v>
+      </c>
+      <c r="E98" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="F98" s="44"/>
+      <c r="G98" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H98" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I98" s="2">
+        <v>6</v>
+      </c>
+      <c r="J98" s="2">
+        <v>4</v>
+      </c>
+      <c r="K98" s="2">
+        <v>6</v>
+      </c>
+      <c r="L98" s="113">
+        <f>AVERAGE(I98:K98)</f>
+        <v>5.333333333333333</v>
+      </c>
+    </row>
+    <row r="99" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B99" s="2">
+        <v>95</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D99" s="103" t="s">
+        <v>55</v>
+      </c>
+      <c r="E99" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="F99" s="107"/>
+      <c r="G99" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H99" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I99" s="2">
+        <v>3</v>
+      </c>
+      <c r="J99" s="2">
+        <v>6</v>
+      </c>
+      <c r="K99" s="2">
+        <v>6</v>
+      </c>
+      <c r="L99" s="112">
+        <f>AVERAGE(I99:K99)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B100" s="2">
+        <v>96</v>
+      </c>
+      <c r="C100" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D89" s="101" t="s">
+      <c r="D100" s="101" t="s">
         <v>45</v>
       </c>
-      <c r="E89" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="F89" s="96" t="s">
+      <c r="E100" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="F100" s="106" t="s">
         <v>47</v>
       </c>
-      <c r="G89" s="2" t="s">
+      <c r="G100" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H89" s="2" t="s">
+      <c r="H100" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I89" s="2">
+      <c r="I100" s="2">
         <v>0</v>
       </c>
-      <c r="J89" s="2">
+      <c r="J100" s="2">
         <v>9</v>
       </c>
-      <c r="K89" s="2">
+      <c r="K100" s="2">
         <v>6</v>
       </c>
-      <c r="L89" s="80">
-        <f>AVERAGE(I89:K89)</f>
+      <c r="L100" s="112">
+        <f>AVERAGE(I100:K100)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B90" s="2"/>
-    </row>
-    <row r="91" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B91" s="2"/>
-    </row>
-    <row r="92" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B92" s="2"/>
-    </row>
-    <row r="93" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B93" s="2"/>
-    </row>
-    <row r="94" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B94" s="2"/>
-    </row>
-    <row r="95" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B95" s="2"/>
-    </row>
-    <row r="96" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B96" s="2"/>
-    </row>
-    <row r="97" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B97" s="2"/>
-    </row>
-    <row r="98" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B98" s="2"/>
-    </row>
-    <row r="99" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B99" s="2"/>
-    </row>
-    <row r="100" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B100" s="2"/>
-    </row>
-    <row r="101" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B101" s="2"/>
-    </row>
-    <row r="102" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B101" s="2">
+        <v>97</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="D101" s="105" t="s">
+        <v>177</v>
+      </c>
+      <c r="E101" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="F101" s="107"/>
+      <c r="G101" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H101" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I101" s="2">
+        <v>4</v>
+      </c>
+      <c r="J101" s="2">
+        <v>0</v>
+      </c>
+      <c r="K101" s="2">
+        <v>9</v>
+      </c>
+      <c r="L101" s="47">
+        <f>AVERAGE(I101:K101)</f>
+        <v>4.333333333333333</v>
+      </c>
+    </row>
+    <row r="102" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B102" s="2"/>
     </row>
-    <row r="103" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B103" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="B5:L89">
-    <sortCondition descending="1" ref="L5:L89"/>
-    <sortCondition ref="E5:E89"/>
-    <sortCondition ref="C5:C89"/>
+  <sortState ref="B5:L101">
+    <sortCondition descending="1" ref="L5:L101"/>
+    <sortCondition ref="E5:E101"/>
+    <sortCondition ref="C5:C101"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>